<commit_message>
Remove hard-coded column names.
</commit_message>
<xml_diff>
--- a/inst/error/Faculty/PROFidA.xlsx
+++ b/inst/error/Faculty/PROFidA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://omunet-my.sharepoint.com/personal/s21413e_omu_ac_jp/Documents/教務委員/Matching/Data4Test1/Faculty/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1684bc3b7bd79ed3/Projects/omueconMatch/inst/error/Faculty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{6CB48D5E-F43F-A344-AB04-6F15F8BA8081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F22B64A-7FFE-5849-AA64-9907C96E7451}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:1_{6CB48D5E-F43F-A344-AB04-6F15F8BA8081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AFA6A5B-C072-C148-A830-AB615F83EEEC}"/>
   <bookViews>
-    <workbookView xWindow="20900" yWindow="3280" windowWidth="25840" windowHeight="17040" activeTab="1" xr2:uid="{56E0F391-1520-9245-91B6-31950EE167B6}"/>
+    <workbookView xWindow="22040" yWindow="3080" windowWidth="16360" windowHeight="17040" activeTab="1" xr2:uid="{56E0F391-1520-9245-91B6-31950EE167B6}"/>
   </bookViews>
   <sheets>
     <sheet name="設定" sheetId="4" r:id="rId1"/>
@@ -818,14 +818,14 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>